<commit_message>
add res for 12155 models
</commit_message>
<xml_diff>
--- a/Results/launch_results.xlsx
+++ b/Results/launch_results.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toaxo\Desktop\MSU\4_1\Hausdorff\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB98DF8-4DAD-4C7F-B138-E3195021D776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3E86CD-C2CA-47EA-B991-21576D4590CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14B6E373-58AE-4468-B41D-449D8FB61223}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{14B6E373-58AE-4468-B41D-449D8FB61223}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="scipy.spatial.distance" sheetId="1" r:id="rId1"/>
+    <sheet name="NaiveHDD" sheetId="4" r:id="rId2"/>
+    <sheet name="EARLYBREAK" sheetId="2" r:id="rId3"/>
+    <sheet name="KDTree" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>PROCESS</t>
   </si>
@@ -53,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -153,10 +156,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -296,7 +299,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sayfa1!$D$3</c:f>
+              <c:f>'scipy.spatial.distance'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -382,7 +385,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sayfa1!$C$4:$C$9</c:f>
+              <c:f>'scipy.spatial.distance'!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -393,7 +396,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
@@ -409,27 +412,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$D$4:$D$9</c:f>
+              <c:f>'scipy.spatial.distance'!$D$4:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2588.0455000000002</c:v>
+                  <c:v>2592.8712799999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2585.17938</c:v>
+                  <c:v>2585.0081500000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1294.74784</c:v>
+                  <c:v>870.88338999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>382.55266999999998</c:v>
+                  <c:v>394.28219999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>193.46599000000001</c:v>
+                  <c:v>189.33671000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96.829220000000007</c:v>
+                  <c:v>94.524259999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,7 +464,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sayfa1!$E$3</c:f>
+              <c:f>'scipy.spatial.distance'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -558,7 +561,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$E$4:$E$9</c:f>
+              <c:f>'scipy.spatial.distance'!$E$4:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -566,19 +569,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0011086735497636</c:v>
+                  <c:v>1.0030418201969691</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9988799517904585</c:v>
+                  <c:v>2.9772887045187528</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7652004624618103</c:v>
+                  <c:v>6.576181425385168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.377263362930094</c:v>
+                  <c:v>13.694498441427443</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.72793914894698</c:v>
+                  <c:v>27.430749312398742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,7 +1094,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sayfa1!$D$26</c:f>
+              <c:f>'scipy.spatial.distance'!$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1197,7 +1200,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sayfa1!$C$27:$C$32</c:f>
+              <c:f>'scipy.spatial.distance'!$C$27:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1224,7 +1227,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$D$27:$D$32</c:f>
+              <c:f>'scipy.spatial.distance'!$D$27:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1275,7 +1278,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sayfa1!$E$26</c:f>
+              <c:f>'scipy.spatial.distance'!$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1373,7 +1376,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$E$27:$E$32</c:f>
+              <c:f>'scipy.spatial.distance'!$E$27:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2931,16 +2934,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>308161</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>599514</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>124386</xdr:rowOff>
+      <xdr:rowOff>169210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>224118</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>515470</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>89648</xdr:rowOff>
+      <xdr:rowOff>134472</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3267,21 +3270,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA839B1C-3EAE-4507-A101-468001B68762}">
   <dimension ref="C2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="3" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="3:5" ht="21" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
@@ -3298,11 +3300,11 @@
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
-        <v>2588.0455000000002</v>
+      <c r="D4" s="5">
+        <v>2592.8712799999998</v>
       </c>
       <c r="E4" s="4">
-        <f>$D$4/D4</f>
+        <f t="shared" ref="E4:E9" si="0">$D$4/D4</f>
         <v>1</v>
       </c>
     </row>
@@ -3310,67 +3312,69 @@
       <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
-        <v>2585.17938</v>
+      <c r="D5" s="5">
+        <v>2585.0081500000001</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:E9" si="0">$D$4/D5</f>
-        <v>1.0011086735497636</v>
+        <f t="shared" si="0"/>
+        <v>1.0030418201969691</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1294.74784</v>
+        <v>4</v>
+      </c>
+      <c r="D6" s="5">
+        <v>870.88338999999996</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1.9988799517904585</v>
+        <v>2.9772887045187528</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <v>8</v>
       </c>
-      <c r="D7" s="6">
-        <v>382.55266999999998</v>
+      <c r="D7" s="5">
+        <v>394.28219999999999</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>6.7652004624618103</v>
+        <v>6.576181425385168</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <v>16</v>
       </c>
-      <c r="D8" s="6">
-        <v>193.46599000000001</v>
+      <c r="D8" s="5">
+        <v>189.33671000000001</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>13.377263362930094</v>
+        <v>13.694498441427443</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>32</v>
       </c>
-      <c r="D9" s="6">
-        <v>96.829220000000007</v>
+      <c r="D9" s="5">
+        <v>94.524259999999998</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>26.72793914894698</v>
+        <v>27.430749312398742</v>
       </c>
     </row>
+    <row r="22" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="3:5" ht="21" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
@@ -3387,11 +3391,11 @@
       <c r="C27" s="2">
         <v>1</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>6784.8931700000003</v>
       </c>
       <c r="E27" s="4">
-        <f>$D$27/D27</f>
+        <f t="shared" ref="E27:E32" si="1">$D$27/D27</f>
         <v>1</v>
       </c>
     </row>
@@ -3399,11 +3403,11 @@
       <c r="C28" s="2">
         <v>2</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>3472.13913</v>
       </c>
       <c r="E28" s="4">
-        <f>$D$27/D28</f>
+        <f t="shared" si="1"/>
         <v>1.9540959955714678</v>
       </c>
     </row>
@@ -3411,11 +3415,11 @@
       <c r="C29" s="2">
         <v>4</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>1782.1538499999999</v>
       </c>
       <c r="E29" s="4">
-        <f>$D$27/D29</f>
+        <f t="shared" si="1"/>
         <v>3.8071310005025665</v>
       </c>
     </row>
@@ -3423,11 +3427,11 @@
       <c r="C30" s="2">
         <v>8</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>951.96270000000004</v>
       </c>
       <c r="E30" s="4">
-        <f>$D$27/D30</f>
+        <f t="shared" si="1"/>
         <v>7.1272678750963667</v>
       </c>
     </row>
@@ -3435,11 +3439,11 @@
       <c r="C31" s="2">
         <v>16</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>504.84285999999997</v>
       </c>
       <c r="E31" s="4">
-        <f>$D$27/D31</f>
+        <f t="shared" si="1"/>
         <v>13.439614001869812</v>
       </c>
     </row>
@@ -3447,11 +3451,11 @@
       <c r="C32" s="2">
         <v>32</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>290.83019000000002</v>
       </c>
       <c r="E32" s="4">
-        <f>$D$27/D32</f>
+        <f t="shared" si="1"/>
         <v>23.329397714865845</v>
       </c>
     </row>
@@ -3464,4 +3468,184 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7133C0AE-F16D-48E6-B7D2-D067ED4DDD94}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58481C45-4010-45FD-AA67-D1CD08F55204}">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="2:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>26214.107189999999</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5">
+        <v>17597.07388</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA68C7D0-61C1-475D-9777-CB4211107AD9}">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5">
+        <v>35200.117259999999</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5">
+        <v>21575.88726</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
code beauty and add new results
</commit_message>
<xml_diff>
--- a/Results/launch_results.xlsx
+++ b/Results/launch_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toaxo\Desktop\MSU\4_1\Hausdorff\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC5B0B6-0248-463E-98FB-6FFFE2A60EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6749DC0F-2A90-4284-8240-58A3B1DF1ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{14B6E373-58AE-4468-B41D-449D8FB61223}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{14B6E373-58AE-4468-B41D-449D8FB61223}"/>
   </bookViews>
   <sheets>
     <sheet name="scipy.spatial.distance 12155" sheetId="1" r:id="rId1"/>
@@ -4139,7 +4139,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'EARLYBREAK 1K'!$D$7</c:f>
+              <c:f>'scipy.spatial.KDTree 1K'!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4263,7 +4263,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'EARLYBREAK 1K'!$D$8:$D$13</c:f>
+              <c:f>'scipy.spatial.KDTree 1K'!$D$8:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4271,19 +4271,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0003691040022635</c:v>
+                  <c:v>0.98473089676822723</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9940444664481465</c:v>
+                  <c:v>2.9792992235827613</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4627294463866445</c:v>
+                  <c:v>6.7979950134351945</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9794865663558721</c:v>
+                  <c:v>13.609319753258459</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.861529761968592</c:v>
+                  <c:v>22.928889248372148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14158,8 +14158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA68C7D0-61C1-475D-9777-CB4211107AD9}">
   <dimension ref="B5:E32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14447,8 +14447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58481C45-4010-45FD-AA67-D1CD08F55204}">
   <dimension ref="B5:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14737,7 +14737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7133C0AE-F16D-48E6-B7D2-D067ED4DDD94}">
   <dimension ref="B5:E32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>